<commit_message>
Add updated class diagram and parttype enum. rework input to accept whole sentences, not just words. add a few report functionalities.
</commit_message>
<xml_diff>
--- a/Auto_scrum.xlsx
+++ b/Auto_scrum.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23500" windowHeight="15640" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sample" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 01 Backlog" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 02 Backlog" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
   <si>
     <t>Product Name:</t>
   </si>
@@ -415,6 +416,30 @@
   </si>
   <si>
     <t>Upload all diagrams to computer</t>
+  </si>
+  <si>
+    <t>change to_string() methods to &lt;&lt; overide</t>
+  </si>
+  <si>
+    <t>This will take time</t>
+  </si>
+  <si>
+    <t>sick</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>write create_model() function</t>
+  </si>
+  <si>
+    <t>Controller.cpp</t>
+  </si>
+  <si>
+    <t>Create part type header file</t>
+  </si>
+  <si>
+    <t>add part type to uml diagram</t>
   </si>
 </sst>
 </file>
@@ -1069,13 +1094,13 @@
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1234,6 +1259,245 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 02 Backlog'!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2058559040"/>
+        <c:axId val="-2065878176"/>
+      </c:lineChart>
+      <c:valAx>
+        <c:axId val="-2065878176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2058559040"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2058559040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2065878176"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
@@ -1300,6 +1564,39 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="2565400" y="444500"/>
+    <xdr:ext cx="3751234" cy="1855043"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="shape">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{812657B9-FB79-42B5-BAE2-124EFB8FD54A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="2552700" y="393700"/>
     <xdr:ext cx="3751234" cy="1855043"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1628,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI46"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1639,7 +1936,8 @@
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="7" width="36.1640625" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" customWidth="1"/>
+    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59.5" customWidth="1"/>
     <col min="9" max="1024" width="10.6640625" customWidth="1"/>
   </cols>
@@ -29719,7 +30017,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -29953,16 +30251,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
@@ -30106,7 +30405,7 @@
         <v>85</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -30120,7 +30419,7 @@
         <v>86</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -30134,7 +30433,7 @@
         <v>87</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -30244,7 +30543,7 @@
         <v>99</v>
       </c>
       <c r="G19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
@@ -30468,7 +30767,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>18</v>
       </c>
@@ -30485,7 +30784,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>19</v>
       </c>
@@ -30502,7 +30801,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>20</v>
       </c>
@@ -30519,7 +30818,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>21</v>
       </c>
@@ -30536,7 +30835,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>22</v>
       </c>
@@ -30553,7 +30852,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>23</v>
       </c>
@@ -30570,7 +30869,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>24</v>
       </c>
@@ -30587,7 +30886,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>25</v>
       </c>
@@ -30604,7 +30903,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>26</v>
       </c>
@@ -30621,7 +30920,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>27</v>
       </c>
@@ -30638,7 +30937,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>28</v>
       </c>
@@ -30655,7 +30954,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>29</v>
       </c>
@@ -30672,7 +30971,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>30</v>
       </c>
@@ -30689,7 +30988,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>31</v>
       </c>
@@ -30706,7 +31005,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>32</v>
       </c>
@@ -30721,6 +31020,615 @@
       </c>
       <c r="G47" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>33</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" t="s">
+        <v>126</v>
+      </c>
+      <c r="H48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9">
+        <v>42588</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="9">
+        <v>42595</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="1">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add order creation and fix object slicing problem
</commit_message>
<xml_diff>
--- a/Auto_scrum.xlsx
+++ b/Auto_scrum.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sample" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint 01 Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 02 Backlog" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 03 Backlog" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="138">
   <si>
     <t>Product Name:</t>
   </si>
@@ -440,6 +441,9 @@
   </si>
   <si>
     <t>add part type to uml diagram</t>
+  </si>
+  <si>
+    <t>Auto</t>
   </si>
 </sst>
 </file>
@@ -1498,6 +1502,245 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2025568768"/>
+        <c:axId val="-2025949136"/>
+      </c:lineChart>
+      <c:valAx>
+        <c:axId val="-2025949136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2025568768"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2025568768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2025949136"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
@@ -1597,6 +1840,39 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="2552700" y="393700"/>
+    <xdr:ext cx="3751234" cy="1855043"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="shape">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{812657B9-FB79-42B5-BAE2-124EFB8FD54A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="3225800" y="419100"/>
     <xdr:ext cx="3751234" cy="1855043"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1925,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1946,7 +2222,9 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -29700,6 +29978,9 @@
       <c r="B29">
         <v>1</v>
       </c>
+      <c r="C29" t="s">
+        <v>132</v>
+      </c>
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -29717,6 +29998,9 @@
       <c r="B30">
         <v>2</v>
       </c>
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
       <c r="E30" t="s">
         <v>20</v>
       </c>
@@ -29734,6 +30018,9 @@
       <c r="B31">
         <v>3</v>
       </c>
+      <c r="C31" t="s">
+        <v>132</v>
+      </c>
       <c r="E31" t="s">
         <v>27</v>
       </c>
@@ -29750,6 +30037,9 @@
     <row r="32" spans="1:1023" x14ac:dyDescent="0.15">
       <c r="B32">
         <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>132</v>
       </c>
       <c r="E32" t="s">
         <v>31</v>
@@ -31053,7 +31343,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="H46" sqref="A1:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -31635,4 +31925,519 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="45.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="9">
+        <v>42595</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="9">
+        <v>42602</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="1">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>